<commit_message>
Update sample data to reflect new nested validation structure
Refactor `create_sample_excel` to generate a two-sheet structure for parameter definitions and nested validation rules, supporting AND/OR logic.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 65cb9bd6-52fd-4848-a801-a544d4e30ff2
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
</commit_message>
<xml_diff>
--- a/参数知识库.xlsx
+++ b/参数知识库.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="空域配置" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="参数信息" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="验证规则" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,89 +472,48 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>期望值</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>漏配检查值</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>条件表达式</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
           <t>值描述</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>验证参数列表</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <f>== 配置规则说明 ===</f>
+        <f>== 参数信息表说明 ===</f>
         <v/>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>必填项: MO名称/参数名称/参数ID/参数类型</t>
+          <t>记录所有参数的基本信息，与验证规则表分离</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>参数类型: single(单值)/multiple(多开关)</t>
+          <t>参数类型: single(单值)/multiple(多值开关组合)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>期望值与漏配检查值互斥，二选一填写</t>
+          <t>参数的中文名称，用于验证规则表中引用</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>验证参数列表格式: MO名称:参数名称:期望值;多个用;分隔</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>参数的英文ID，用于生成MOD命令</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>single/multiple，决定验证方式</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>配置规则说明(重点)</t>
+          <t>参数的详细说明和业务含义</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>有值时触发参数值稽核(与漏配检查值二选一)</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>有值时触发漏配检查(与期望值二选一)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>格式:参数名=值,多条件用逗号分隔</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>多值参数开关状态说明</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>格式:MO名称:参数名称:期望值;多个用;分隔
-⚠️关键逻辑:漏配检查通过后自动触发以下验证:
-1. MO名称:定位目标网元数据
-2. 参数名称:定位具体参数
-3. 期望值:验证实际值是否匹配
-示例:NRCELLFREQRELATION:连接态频率优先级:5</t>
+          <t>仅多值参数使用，说明各开关含义</t>
         </is>
       </c>
     </row>
@@ -565,7 +525,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NR DU小区</t>
+          <t>NR DU小区配置</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -590,28 +550,20 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>小区覆盖半径</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+          <t>小区覆盖半径，影响信号覆盖范围</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NRCELL</t>
+          <t>NRDUCELL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NR小区</t>
+          <t>NR DU小区配置</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -621,12 +573,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>跟踪区码</t>
+          <t>最大传输功率</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TrackingAreaCode</t>
+          <t>MaxTxPower</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -636,28 +588,20 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>小区所属跟踪区</t>
+          <t>小区最大传输功率，单位dBm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NRCELLFREQRELATION</t>
+          <t>NRCELL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NR小区频率关系</t>
+          <t>NR小区基本配置</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -667,12 +611,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SSB频域位置</t>
+          <t>跟踪区码</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3001</t>
+          <t>TrackingAreaCode</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -682,22 +626,10 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>SSB的频域位置</t>
+          <t>小区所属跟踪区标识</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>7783</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>NRCELLFREQRELATION:连接态频率优先级:5;NRCELLFREQRELATION:测量频点:38400</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -707,7 +639,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NR小区</t>
+          <t>NR小区基本配置</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -717,12 +649,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>工作带宽</t>
+          <t>小区状态</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OperatingBandwidth</t>
+          <t>CellState</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -732,20 +664,472 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>小区工作带宽</t>
+          <t>小区运行状态：激活/非激活</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NRDUCELLBEAM</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NR DU小区波束配置</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>空域配置</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>波束开关组合</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BeamSwitchCombination</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>multiple</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>多个波束开关的组合状态配置</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>beam1:第1号波束开关状态(开/关); beam2:第2号波束开关状态(开/关); beam3:第3号波束开关状态(开/关)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NRCELLFREQRELATION</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NR小区频率关系配置</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>空域配置</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>连接态频率优先级</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ConnFreqPriority</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>连接态下的频率优先级配置</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>校验ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>校验类型</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MO名称</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>参数名称</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>条件表达式</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>期望值</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>继续校验</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>错误描述</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <f>== 验证规则表说明 ===</f>
+        <v/>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>漏配/错配，每行只能是其中一种</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>目标MO名称，必须在参数信息表中存在</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>目标参数名称，必须在参数信息表中存在</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>筛选条件: (参数名1=值1 and 参数名2=值2) or (参数名3&gt;值3 and 参数名2!=值2)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>单值参数直接填值，多值参数格式: k1:开&amp;k2:关&amp;k3:开</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>下一步校验的校验ID，支持嵌套调用</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>校验失败时的详细描述信息</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MISS_001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>漏配</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NRCELL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>跟踪区码</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>NRDUCELL:最大传输功率:43;NRCELLPDSCH:调制方式:64QAM</t>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ERROR_001</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>缺少跟踪区码为100的小区配置</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ERROR_001</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>错配</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NRDUCELL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>小区半径(米)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>跟踪区码=100</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ERROR_002</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>跟踪区码为100的小区，半径应配置为500米</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ERROR_002</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>错配</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NRDUCELL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>最大传输功率</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>跟踪区码=100 and 小区半径(米)=500</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ERROR_003</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>满足条件的小区，最大传输功率应为43dBm</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ERROR_003</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>错配</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NRDUCELLBEAM</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>波束开关组合</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>(小区半径(米)&gt;=500 and 最大传输功率&gt;=40) or (跟踪区码!=200 and 小区状态=激活)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>beam1:开&amp;beam2:关&amp;beam3:开</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>MISS_002</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>满足功率和覆盖条件时，beam1和beam3应开启，beam2应关闭</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MISS_002</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>漏配</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NRCELLFREQRELATION</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>连接态频率优先级</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>小区状态=激活 and 最大传输功率&gt;40</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ERROR_004</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>激活状态且高功率小区必须配置频率优先级为5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ERROR_004</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>错配</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NRCELL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>小区状态</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>跟踪区码=100 and 连接态频率优先级=5</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>激活</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>配置完整的小区状态必须为激活</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>COMPLEX_001</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>错配</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NRDUCELL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>小区半径(米)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>(跟踪区码=100 and 小区状态=激活) or (跟踪区码=200 and 最大传输功率&gt;45) or (小区状态!=激活 and 连接态频率优先级&gt;=3)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>满足任一复杂条件组合时，小区半径应为800米</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve parameter checking system with nested validation and conditional logic
Refactor ParameterChecker to support complex conditional expressions (AND/OR) for parameter validation, enabling nested checks and improving the handling of single and multiple value parameters.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7be64310-4725-4b58-9ac1-c1dab307d313
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
</commit_message>
<xml_diff>
--- a/参数知识库.xlsx
+++ b/参数知识库.xlsx
@@ -28,17 +28,24 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00366092"/>
+        <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -46,20 +53,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,13 +427,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -477,70 +488,67 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <f>== 参数信息表说明 ===</f>
-        <v/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NRCELL</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>记录所有参数的基本信息，与验证规则表分离</t>
+          <t>5G小区对象</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>参数类型: single(单值)/multiple(多值开关组合)</t>
+          <t>5G基础配置</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>参数的中文名称，用于验证规则表中引用</t>
+          <t>跟踪区码</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>参数的英文ID，用于生成MOD命令</t>
+          <t>tac</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>single/multiple，决定验证方式</t>
+          <t>single</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>参数的详细说明和业务含义</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>仅多值参数使用，说明各开关含义</t>
-        </is>
-      </c>
+          <t>标识小区所属的跟踪区</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NRDUCELL</t>
+          <t>NRCELL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NR DU小区配置</t>
+          <t>5G小区对象</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>空域配置</t>
+          <t>5G基础配置</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>小区半径(米)</t>
+          <t>小区状态</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CellRadius</t>
+          <t>cellState</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -550,7 +558,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>小区覆盖半径，影响信号覆盖范围</t>
+          <t>小区的激活状态</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -563,22 +571,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NR DU小区配置</t>
+          <t>5G DU小区对象</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>空域配置</t>
+          <t>5G物理层配置</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>最大传输功率</t>
+          <t>小区半径(米)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MaxTxPower</t>
+          <t>cellRadius</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -588,7 +596,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>小区最大传输功率，单位dBm</t>
+          <t>小区覆盖半径</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -596,27 +604,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NRCELL</t>
+          <t>NRDUCELL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NR小区基本配置</t>
+          <t>5G DU小区对象</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>空域配置</t>
+          <t>5G物理层配置</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>跟踪区码</t>
+          <t>最大传输功率</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>TrackingAreaCode</t>
+          <t>maxTxPower</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -626,7 +634,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>小区所属跟踪区标识</t>
+          <t>小区最大发射功率</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -634,120 +642,82 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NRCELL</t>
+          <t>NRDUCELLBEAM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NR小区基本配置</t>
+          <t>5G波束配置对象</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>空域配置</t>
+          <t>5G波束管理</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>小区状态</t>
+          <t>波束开关组合</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CellState</t>
+          <t>beamSwitchComb</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>single</t>
+          <t>multiple</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>小区运行状态：激活/非激活</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>波束开关状态组合</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>beam1:第一波束开关,beam2:第二波束开关,beam3:第三波束开关</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NRDUCELLBEAM</t>
+          <t>NRCELLFREQRELATION</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NR DU小区波束配置</t>
+          <t>小区频率关系对象</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>空域配置</t>
+          <t>频率管理配置</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>波束开关组合</t>
+          <t>连接态频率优先级</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BeamSwitchCombination</t>
+          <t>connectedFreqPriority</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>multiple</t>
+          <t>single</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>多个波束开关的组合状态配置</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>beam1:第1号波束开关状态(开/关); beam2:第2号波束开关状态(开/关); beam3:第3号波束开关状态(开/关)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NRCELLFREQRELATION</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NR小区频率关系配置</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>空域配置</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>连接态频率优先级</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ConnFreqPriority</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>single</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>连接态下的频率优先级配置</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>连接态下的频率优先级</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -760,13 +730,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="32" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -786,113 +765,99 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>参数名称</t>
+          <t>条件表达式</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>条件表达式</t>
+          <t>期望值表达式</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>期望值</t>
+          <t>错误描述</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>继续校验</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>错误描述</t>
+          <t>继续校验ID</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <f>== 验证规则表说明 ===</f>
-        <v/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MISS_001</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>漏配/错配，每行只能是其中一种</t>
+          <t>漏配</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>目标MO名称，必须在参数信息表中存在</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>目标参数名称，必须在参数信息表中存在</t>
-        </is>
-      </c>
+          <t>NRCELL</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>筛选条件: (参数名1=值1 and 参数名2=值2) or (参数名3&gt;值3 and 参数名2!=值2)</t>
+          <t>跟踪区码=100</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>单值参数直接填值，多值参数格式: k1:开&amp;k2:关&amp;k3:开</t>
+          <t>缺少跟踪区码为100的小区配置</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>下一步校验的校验ID，支持嵌套调用</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>校验失败时的详细描述信息</t>
+          <t>ERROR_001</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MISS_001</t>
+          <t>ERROR_001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>漏配</t>
+          <t>错配</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NRCELL</t>
+          <t>NRDUCELL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>跟踪区码</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>跟踪区码=100</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>小区半径(米)=500</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>跟踪区码为100的小区，半径应配置为500米</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ERROR_001</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>缺少跟踪区码为100的小区配置</t>
+          <t>ERROR_002</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ERROR_001</t>
+          <t>ERROR_002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -907,34 +872,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>小区半径(米)</t>
+          <t>跟踪区码=100and小区半径(米)=500</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>跟踪区码=100</t>
+          <t>最大传输功率=43</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>半径500米的小区，功率应为43dBm</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ERROR_002</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>跟踪区码为100的小区，半径应配置为500米</t>
+          <t>ERROR_003</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ERROR_002</t>
+          <t>ERROR_003</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -944,123 +904,104 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NRDUCELL</t>
+          <t>NRDUCELLBEAM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>最大传输功率</t>
+          <t>跟踪区码=100</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>跟踪区码=100 and 小区半径(米)=500</t>
+          <t>波束开关组合=beam1:开&amp;beam2:关&amp;beam3:开</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>跟踪区码100的小区，波束组合应为beam1开beam2关beam3开</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ERROR_003</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>满足条件的小区，最大传输功率应为43dBm</t>
+          <t>MISS_002</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ERROR_003</t>
+          <t>MISS_002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>错配</t>
+          <t>漏配</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NRDUCELLBEAM</t>
+          <t>NRCELLFREQRELATION</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>波束开关组合</t>
+          <t>跟踪区码=100</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(小区半径(米)&gt;=500 and 最大传输功率&gt;=40) or (跟踪区码!=200 and 小区状态=激活)</t>
+          <t>连接态频率优先级=1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>beam1:开&amp;beam2:关&amp;beam3:开</t>
+          <t>缺少跟踪区码100小区的频率优先级配置</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>MISS_002</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>满足功率和覆盖条件时，beam1和beam3应开启，beam2应关闭</t>
+          <t>ERROR_004</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MISS_002</t>
+          <t>ERROR_004</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>漏配</t>
+          <t>错配</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NRCELLFREQRELATION</t>
+          <t>NRCELL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>连接态频率优先级</t>
+          <t>跟踪区码=100and连接态频率优先级=1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>小区状态=激活 and 最大传输功率&gt;40</t>
+          <t>小区状态=激活</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>ERROR_004</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>激活状态且高功率小区必须配置频率优先级为5</t>
-        </is>
-      </c>
+          <t>已配置频率优先级的小区状态应为激活</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ERROR_004</t>
+          <t>COMPLEX_001</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1070,68 +1011,58 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NRCELL</t>
+          <t>NRDUCELL</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>小区状态</t>
+          <t>(跟踪区码=200or跟踪区码=300)and小区状态=激活</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>跟踪区码=100 and 连接态频率优先级=5</t>
+          <t>小区半径(米)=1000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>激活</t>
+          <t>特殊跟踪区的激活小区半径应为1000米</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>配置完整的小区状态必须为激活</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>COMPLEX_001</t>
+          <t>COMPLEX_002</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>错配</t>
+          <t>漏配</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>NRDUCELL</t>
+          <t>NRCELL</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>小区半径(米)</t>
+          <t>小区半径(米)&gt;500and最大传输功率&gt;=40</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(跟踪区码=100 and 小区状态=激活) or (跟踪区码=200 and 最大传输功率&gt;45) or (小区状态!=激活 and 连接态频率优先级&gt;=3)</t>
+          <t>小区状态=激活</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>大半径高功率小区必须激活</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>满足任一复杂条件组合时，小区半径应为800米</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>